<commit_message>
updated community day presentation
</commit_message>
<xml_diff>
--- a/docs/label_distribution.xlsx
+++ b/docs/label_distribution.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\git\drone_steering\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A87E69-6055-4C6C-BCFE-A694802C28E7}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F47247-6207-4FA4-A2BA-3A50BEBFEF5B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11850" xr2:uid="{62938B20-6BFE-4833-95AF-644A79547EEB}"/>
   </bookViews>
@@ -33,9 +33,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>No movement</t>
-  </si>
-  <si>
     <t>Take-off</t>
   </si>
   <si>
@@ -52,6 +49,9 @@
   </si>
   <si>
     <t>Land</t>
+  </si>
+  <si>
+    <t>No gesture</t>
   </si>
 </sst>
 </file>
@@ -196,7 +196,7 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>No movement</c:v>
+                  <c:v>No gesture</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Take-off</c:v>
@@ -1262,8 +1262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F491855-1948-4BA0-94A3-A028B35420D5}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1273,7 +1273,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1">
         <v>13894</v>
@@ -1281,7 +1281,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>701</v>
@@ -1289,7 +1289,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>576</v>
@@ -1297,7 +1297,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>991</v>
@@ -1305,7 +1305,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>677</v>
@@ -1313,7 +1313,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>660</v>
@@ -1321,7 +1321,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>689</v>

</xml_diff>